<commit_message>
Merge offer price template
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/OfferPriceExportTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/OfferPriceExportTemplate.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19155" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="2595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>${offerItem.typeOfService}</t>
   </si>
@@ -31,9 +27,6 @@
   </si>
   <si>
     <t>${offerItem.feeUnitId}</t>
-  </si>
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
   </si>
   <si>
     <t>${offerItem.currencyUnit}</t>
@@ -145,10 +138,7 @@
     <t>STT</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${offerItems}" var="offerItem" varStatus="status"&gt;</t>
-  </si>
-  <si>
-    <t>${status.index}</t>
+    <t>${offerItem.index}</t>
   </si>
 </sst>
 </file>
@@ -301,17 +291,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -325,6 +309,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,282 +684,264 @@
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="3" t="s">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F2" s="4" t="s">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F3" s="4" t="s">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F4" s="4" t="s">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+    <row r="22" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>